<commit_message>
update 0.0.2 version setup.py
</commit_message>
<xml_diff>
--- a/docs/template.xlsx
+++ b/docs/template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/PycharmProjects/azkaban_excel_yaml/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7DC50C-097D-3D4C-BB29-E45F7A36251D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="3"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -24,7 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ora2pg!$A$1:$I$100</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">pg2mongo!$A$1:$I$74</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -63,6 +69,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -73,6 +80,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -85,6 +93,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -95,6 +104,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -107,6 +117,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -117,6 +128,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -129,6 +141,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -139,6 +152,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -1191,15 +1205,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm:ss;@"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1211,6 +1221,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1218,6 +1229,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1225,6 +1237,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1232,14 +1245,7 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1248,147 +1254,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="9"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1401,194 +1279,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1701,251 +1393,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1972,39 +1422,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2023,71 +1454,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2345,215 +1748,210 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11" style="17"/>
-    <col min="2" max="2" width="8.16666666666667" style="18" customWidth="1"/>
-    <col min="3" max="3" width="84.8333333333333" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="18"/>
+    <col min="1" max="1" width="11" style="15"/>
+    <col min="2" max="2" width="8.1640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="84.83203125" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45" customHeight="1" spans="1:4">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:4" ht="45" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" ht="44" customHeight="1" spans="1:4">
-      <c r="A2" s="22" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+    </row>
+    <row r="2" spans="1:4" ht="44" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-    </row>
-    <row r="4" ht="15.6" spans="1:4">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" ht="16">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="110.4" spans="1:4">
-      <c r="A5" s="29">
+    <row r="5" spans="1:4" ht="128">
+      <c r="A5" s="22">
         <v>1</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="27">
         <v>44463</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="29"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="29"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="29"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="29"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="29"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="13.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="27.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:5">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="16">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://192.168.31.36:18443/" tooltip="https://192.168.31.36:18443/"/>
-  </hyperlinks>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8333333333333" defaultRowHeight="13.8" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.8333333333333" customWidth="1"/>
-    <col min="2" max="2" width="15.1666666666667" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:2" ht="16">
+      <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2563,45 +1961,44 @@
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="57.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.83203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2635,7 +2032,7 @@
       <c r="B2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="35" t="str">
+      <c r="C2" s="28" t="str">
         <f>G2&amp;" "&amp;F2&amp;" "&amp;E2&amp;" ? * *"</f>
         <v>0 10 0 ? * *</v>
       </c>
@@ -2659,7 +2056,7 @@
       <c r="B3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="35" t="str">
+      <c r="C3" s="28" t="str">
         <f t="shared" ref="C3:C66" si="0">G3&amp;" "&amp;F3&amp;" "&amp;E3&amp;" ? * *"</f>
         <v>0 10 0 ? * *</v>
       </c>
@@ -2683,7 +2080,7 @@
       <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="35" t="str">
+      <c r="C4" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 11 0 ? * *</v>
       </c>
@@ -2708,7 +2105,7 @@
       <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="35" t="str">
+      <c r="C5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 11 0 ? * *</v>
       </c>
@@ -2733,7 +2130,7 @@
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="35" t="str">
+      <c r="C6" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 12 0 ? * *</v>
       </c>
@@ -2758,7 +2155,7 @@
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="35" t="str">
+      <c r="C7" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 12 0 ? * *</v>
       </c>
@@ -2783,7 +2180,7 @@
       <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="35" t="str">
+      <c r="C8" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 13 0 ? * *</v>
       </c>
@@ -2808,7 +2205,7 @@
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="35" t="str">
+      <c r="C9" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 13 0 ? * *</v>
       </c>
@@ -2833,7 +2230,7 @@
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="35" t="str">
+      <c r="C10" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 14 0 ? * *</v>
       </c>
@@ -2858,7 +2255,7 @@
       <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="35" t="str">
+      <c r="C11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 14 0 ? * *</v>
       </c>
@@ -2883,7 +2280,7 @@
       <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="35" t="str">
+      <c r="C12" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 15 0 ? * *</v>
       </c>
@@ -2908,7 +2305,7 @@
       <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="35" t="str">
+      <c r="C13" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 15 0 ? * *</v>
       </c>
@@ -2933,7 +2330,7 @@
       <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="35" t="str">
+      <c r="C14" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 16 0 ? * *</v>
       </c>
@@ -2958,7 +2355,7 @@
       <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="35" t="str">
+      <c r="C15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 16 0 ? * *</v>
       </c>
@@ -2983,7 +2380,7 @@
       <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="35" t="str">
+      <c r="C16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 17 0 ? * *</v>
       </c>
@@ -3008,7 +2405,7 @@
       <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="35" t="str">
+      <c r="C17" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 17 0 ? * *</v>
       </c>
@@ -3033,7 +2430,7 @@
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="35" t="str">
+      <c r="C18" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 18 0 ? * *</v>
       </c>
@@ -3058,7 +2455,7 @@
       <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="35" t="str">
+      <c r="C19" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 18 0 ? * *</v>
       </c>
@@ -3083,7 +2480,7 @@
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="35" t="str">
+      <c r="C20" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 19 0 ? * *</v>
       </c>
@@ -3108,7 +2505,7 @@
       <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="35" t="str">
+      <c r="C21" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 19 0 ? * *</v>
       </c>
@@ -3133,7 +2530,7 @@
       <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="35" t="str">
+      <c r="C22" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 20 0 ? * *</v>
       </c>
@@ -3158,7 +2555,7 @@
       <c r="B23" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="35" t="str">
+      <c r="C23" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 20 0 ? * *</v>
       </c>
@@ -3183,7 +2580,7 @@
       <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="35" t="str">
+      <c r="C24" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 21 0 ? * *</v>
       </c>
@@ -3208,7 +2605,7 @@
       <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="35" t="str">
+      <c r="C25" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 21 0 ? * *</v>
       </c>
@@ -3233,7 +2630,7 @@
       <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="35" t="str">
+      <c r="C26" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 22 0 ? * *</v>
       </c>
@@ -3258,7 +2655,7 @@
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="35" t="str">
+      <c r="C27" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 22 0 ? * *</v>
       </c>
@@ -3283,7 +2680,7 @@
       <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="35" t="str">
+      <c r="C28" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 23 0 ? * *</v>
       </c>
@@ -3308,7 +2705,7 @@
       <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="35" t="str">
+      <c r="C29" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 23 0 ? * *</v>
       </c>
@@ -3333,7 +2730,7 @@
       <c r="B30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="35" t="str">
+      <c r="C30" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 24 0 ? * *</v>
       </c>
@@ -3358,7 +2755,7 @@
       <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="35" t="str">
+      <c r="C31" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 24 0 ? * *</v>
       </c>
@@ -3383,7 +2780,7 @@
       <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="35" t="str">
+      <c r="C32" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 25 0 ? * *</v>
       </c>
@@ -3408,7 +2805,7 @@
       <c r="B33" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="35" t="str">
+      <c r="C33" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 10 0 ? * *</v>
       </c>
@@ -3432,7 +2829,7 @@
       <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="35" t="str">
+      <c r="C34" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 26 0 ? * *</v>
       </c>
@@ -3457,7 +2854,7 @@
       <c r="B35" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="35" t="str">
+      <c r="C35" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 10 0 ? * *</v>
       </c>
@@ -3481,7 +2878,7 @@
       <c r="B36" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="35" t="str">
+      <c r="C36" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 10 0 ? * *</v>
       </c>
@@ -3505,7 +2902,7 @@
       <c r="B37" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="35" t="str">
+      <c r="C37" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 11 0 ? * *</v>
       </c>
@@ -3530,7 +2927,7 @@
       <c r="B38" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="35" t="str">
+      <c r="C38" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 11 0 ? * *</v>
       </c>
@@ -3555,7 +2952,7 @@
       <c r="B39" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="35" t="str">
+      <c r="C39" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 12 0 ? * *</v>
       </c>
@@ -3566,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="F39:F55" si="2">F37+1</f>
+        <f t="shared" ref="F39:F53" si="2">F37+1</f>
         <v>12</v>
       </c>
       <c r="G39">
@@ -3580,7 +2977,7 @@
       <c r="B40" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="35" t="str">
+      <c r="C40" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 12 0 ? * *</v>
       </c>
@@ -3605,7 +3002,7 @@
       <c r="B41" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="35" t="str">
+      <c r="C41" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 13 0 ? * *</v>
       </c>
@@ -3630,7 +3027,7 @@
       <c r="B42" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="35" t="str">
+      <c r="C42" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 13 0 ? * *</v>
       </c>
@@ -3655,7 +3052,7 @@
       <c r="B43" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="35" t="str">
+      <c r="C43" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 14 0 ? * *</v>
       </c>
@@ -3680,7 +3077,7 @@
       <c r="B44" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="35" t="str">
+      <c r="C44" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 14 0 ? * *</v>
       </c>
@@ -3705,7 +3102,7 @@
       <c r="B45" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="35" t="str">
+      <c r="C45" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 15 0 ? * *</v>
       </c>
@@ -3730,7 +3127,7 @@
       <c r="B46" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="35" t="str">
+      <c r="C46" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 15 0 ? * *</v>
       </c>
@@ -3755,7 +3152,7 @@
       <c r="B47" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="35" t="str">
+      <c r="C47" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 16 0 ? * *</v>
       </c>
@@ -3780,7 +3177,7 @@
       <c r="B48" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="35" t="str">
+      <c r="C48" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 16 0 ? * *</v>
       </c>
@@ -3805,7 +3202,7 @@
       <c r="B49" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="35" t="str">
+      <c r="C49" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 17 0 ? * *</v>
       </c>
@@ -3830,7 +3227,7 @@
       <c r="B50" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="35" t="str">
+      <c r="C50" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 17 0 ? * *</v>
       </c>
@@ -3855,7 +3252,7 @@
       <c r="B51" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="35" t="str">
+      <c r="C51" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 18 0 ? * *</v>
       </c>
@@ -3880,7 +3277,7 @@
       <c r="B52" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="35" t="str">
+      <c r="C52" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 18 0 ? * *</v>
       </c>
@@ -3905,7 +3302,7 @@
       <c r="B53" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C53" s="35" t="str">
+      <c r="C53" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 19 0 ? * *</v>
       </c>
@@ -3930,7 +3327,7 @@
       <c r="B54" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="35" t="str">
+      <c r="C54" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 30 0 ? * *</v>
       </c>
@@ -3954,7 +3351,7 @@
       <c r="B55" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="35" t="str">
+      <c r="C55" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 31 0 ? * *</v>
       </c>
@@ -3978,7 +3375,7 @@
       <c r="B56" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="35" t="str">
+      <c r="C56" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 32 0 ? * *</v>
       </c>
@@ -4002,7 +3399,7 @@
       <c r="B57" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="35" t="str">
+      <c r="C57" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 33 0 ? * *</v>
       </c>
@@ -4026,7 +3423,7 @@
       <c r="B58" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="35" t="str">
+      <c r="C58" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 34 0 ? * *</v>
       </c>
@@ -4050,7 +3447,7 @@
       <c r="B59" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="35" t="str">
+      <c r="C59" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 35 0 ? * *</v>
       </c>
@@ -4074,7 +3471,7 @@
       <c r="B60" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="35" t="str">
+      <c r="C60" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 36 0 ? * *</v>
       </c>
@@ -4098,7 +3495,7 @@
       <c r="B61" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="35" t="str">
+      <c r="C61" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 37 0 ? * *</v>
       </c>
@@ -4122,7 +3519,7 @@
       <c r="B62" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="35" t="str">
+      <c r="C62" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 38 0 ? * *</v>
       </c>
@@ -4146,7 +3543,7 @@
       <c r="B63" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="35" t="str">
+      <c r="C63" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 39 0 ? * *</v>
       </c>
@@ -4170,7 +3567,7 @@
       <c r="B64" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="35" t="str">
+      <c r="C64" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 40 0 ? * *</v>
       </c>
@@ -4194,7 +3591,7 @@
       <c r="B65" t="s">
         <v>97</v>
       </c>
-      <c r="C65" s="35" t="str">
+      <c r="C65" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 41 0 ? * *</v>
       </c>
@@ -4218,7 +3615,7 @@
       <c r="B66" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="35" t="str">
+      <c r="C66" s="28" t="str">
         <f t="shared" si="0"/>
         <v>0 42 0 ? * *</v>
       </c>
@@ -4242,7 +3639,7 @@
       <c r="B67" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="35" t="str">
+      <c r="C67" s="28" t="str">
         <f t="shared" ref="C67:C104" si="3">G67&amp;" "&amp;F67&amp;" "&amp;E67&amp;" ? * *"</f>
         <v>0 43 0 ? * *</v>
       </c>
@@ -4266,7 +3663,7 @@
       <c r="B68" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="35" t="str">
+      <c r="C68" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 44 0 ? * *</v>
       </c>
@@ -4290,7 +3687,7 @@
       <c r="B69" t="s">
         <v>101</v>
       </c>
-      <c r="C69" s="35" t="str">
+      <c r="C69" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 45 0 ? * *</v>
       </c>
@@ -4314,7 +3711,7 @@
       <c r="B70" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="35" t="str">
+      <c r="C70" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 46 0 ? * *</v>
       </c>
@@ -4338,7 +3735,7 @@
       <c r="B71" t="s">
         <v>103</v>
       </c>
-      <c r="C71" s="35" t="str">
+      <c r="C71" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 47 0 ? * *</v>
       </c>
@@ -4362,7 +3759,7 @@
       <c r="B72" t="s">
         <v>104</v>
       </c>
-      <c r="C72" s="35" t="str">
+      <c r="C72" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 48 0 ? * *</v>
       </c>
@@ -4386,7 +3783,7 @@
       <c r="B73" t="s">
         <v>105</v>
       </c>
-      <c r="C73" s="35" t="str">
+      <c r="C73" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 49 0 ? * *</v>
       </c>
@@ -4410,7 +3807,7 @@
       <c r="B74" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="35" t="str">
+      <c r="C74" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 50 0 ? * *</v>
       </c>
@@ -4434,7 +3831,7 @@
       <c r="B75" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="35" t="str">
+      <c r="C75" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 30 0 ? * *</v>
       </c>
@@ -4458,7 +3855,7 @@
       <c r="B76" t="s">
         <v>108</v>
       </c>
-      <c r="C76" s="35" t="str">
+      <c r="C76" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 30 0 ? * *</v>
       </c>
@@ -4482,7 +3879,7 @@
       <c r="B77" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="35" t="str">
+      <c r="C77" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 32 0 ? * *</v>
       </c>
@@ -4506,7 +3903,7 @@
       <c r="B78" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="35" t="str">
+      <c r="C78" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 34 0 ? * *</v>
       </c>
@@ -4530,7 +3927,7 @@
       <c r="B79" t="s">
         <v>111</v>
       </c>
-      <c r="C79" s="35" t="str">
+      <c r="C79" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 36 0 ? * *</v>
       </c>
@@ -4554,7 +3951,7 @@
       <c r="B80" t="s">
         <v>112</v>
       </c>
-      <c r="C80" s="35" t="str">
+      <c r="C80" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 38 0 ? * *</v>
       </c>
@@ -4578,7 +3975,7 @@
       <c r="B81" t="s">
         <v>113</v>
       </c>
-      <c r="C81" s="35" t="str">
+      <c r="C81" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 40 0 ? * *</v>
       </c>
@@ -4602,7 +3999,7 @@
       <c r="B82" t="s">
         <v>114</v>
       </c>
-      <c r="C82" s="35" t="str">
+      <c r="C82" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 42 0 ? * *</v>
       </c>
@@ -4626,7 +4023,7 @@
       <c r="B83" t="s">
         <v>115</v>
       </c>
-      <c r="C83" s="35" t="str">
+      <c r="C83" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 44 0 ? * *</v>
       </c>
@@ -4650,7 +4047,7 @@
       <c r="B84" t="s">
         <v>116</v>
       </c>
-      <c r="C84" s="35" t="str">
+      <c r="C84" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 46 0 ? * *</v>
       </c>
@@ -4674,7 +4071,7 @@
       <c r="B85" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C85" s="35" t="str">
+      <c r="C85" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 30 0 ? * *</v>
       </c>
@@ -4698,7 +4095,7 @@
       <c r="B86" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="35" t="str">
+      <c r="C86" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 40 0 ? * *</v>
       </c>
@@ -4722,7 +4119,7 @@
       <c r="B87" t="s">
         <v>119</v>
       </c>
-      <c r="C87" s="35" t="str">
+      <c r="C87" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 41 0 ? * *</v>
       </c>
@@ -4746,7 +4143,7 @@
       <c r="B88" t="s">
         <v>120</v>
       </c>
-      <c r="C88" s="35" t="str">
+      <c r="C88" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 42 0 ? * *</v>
       </c>
@@ -4770,7 +4167,7 @@
       <c r="B89" t="s">
         <v>121</v>
       </c>
-      <c r="C89" s="35" t="str">
+      <c r="C89" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 43 0 ? * *</v>
       </c>
@@ -4794,7 +4191,7 @@
       <c r="B90" t="s">
         <v>122</v>
       </c>
-      <c r="C90" s="35" t="str">
+      <c r="C90" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 44 0 ? * *</v>
       </c>
@@ -4818,7 +4215,7 @@
       <c r="B91" t="s">
         <v>123</v>
       </c>
-      <c r="C91" s="35" t="str">
+      <c r="C91" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 45 0 ? * *</v>
       </c>
@@ -4842,7 +4239,7 @@
       <c r="B92" t="s">
         <v>124</v>
       </c>
-      <c r="C92" s="35" t="str">
+      <c r="C92" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 46 0 ? * *</v>
       </c>
@@ -4866,7 +4263,7 @@
       <c r="B93" t="s">
         <v>125</v>
       </c>
-      <c r="C93" s="35" t="str">
+      <c r="C93" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 47 0 ? * *</v>
       </c>
@@ -4890,7 +4287,7 @@
       <c r="B94" t="s">
         <v>126</v>
       </c>
-      <c r="C94" s="35" t="str">
+      <c r="C94" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 48 0 ? * *</v>
       </c>
@@ -4914,7 +4311,7 @@
       <c r="B95" t="s">
         <v>127</v>
       </c>
-      <c r="C95" s="35" t="str">
+      <c r="C95" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 49 0 ? * *</v>
       </c>
@@ -4938,7 +4335,7 @@
       <c r="B96" t="s">
         <v>128</v>
       </c>
-      <c r="C96" s="35" t="str">
+      <c r="C96" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 50 0 ? * *</v>
       </c>
@@ -4962,7 +4359,7 @@
       <c r="B97" t="s">
         <v>129</v>
       </c>
-      <c r="C97" s="35" t="str">
+      <c r="C97" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 51 0 ? * *</v>
       </c>
@@ -4986,7 +4383,7 @@
       <c r="B98" t="s">
         <v>130</v>
       </c>
-      <c r="C98" s="35" t="str">
+      <c r="C98" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 52 0 ? * *</v>
       </c>
@@ -5010,7 +4407,7 @@
       <c r="B99" t="s">
         <v>131</v>
       </c>
-      <c r="C99" s="35" t="str">
+      <c r="C99" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 53 0 ? * *</v>
       </c>
@@ -5034,7 +4431,7 @@
       <c r="B100" t="s">
         <v>132</v>
       </c>
-      <c r="C100" s="35" t="str">
+      <c r="C100" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 54 0 ? * *</v>
       </c>
@@ -5058,7 +4455,7 @@
       <c r="B101" t="s">
         <v>133</v>
       </c>
-      <c r="C101" s="35" t="str">
+      <c r="C101" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 55 0 ? * *</v>
       </c>
@@ -5082,7 +4479,7 @@
       <c r="B102" t="s">
         <v>134</v>
       </c>
-      <c r="C102" s="35" t="str">
+      <c r="C102" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 56 0 ? * *</v>
       </c>
@@ -5106,7 +4503,7 @@
       <c r="B103" t="s">
         <v>135</v>
       </c>
-      <c r="C103" s="35" t="str">
+      <c r="C103" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 57 0 ? * *</v>
       </c>
@@ -5130,7 +4527,7 @@
       <c r="B104" t="s">
         <v>136</v>
       </c>
-      <c r="C104" s="35" t="str">
+      <c r="C104" s="28" t="str">
         <f t="shared" si="3"/>
         <v>0 40 0 ? * *</v>
       </c>
@@ -5148,37 +4545,36 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D104">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D104" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.8333333333333" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="39.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="39.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="44.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="37.8333333333333" customWidth="1"/>
-    <col min="6" max="6" width="12.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="9.83333333333333" customWidth="1"/>
-    <col min="8" max="8" width="82.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="255.833333333333" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="82.33203125" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5210,7 +4606,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
@@ -5254,7 +4650,7 @@
         <v>ora2pg_jydb_deleterec</v>
       </c>
     </row>
-    <row r="4" s="11" customFormat="1" spans="1:9">
+    <row r="4" spans="1:9" s="11" customFormat="1">
       <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
@@ -5301,7 +4697,7 @@
         <v>ora2pg_ct_systemconst</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
@@ -5345,7 +4741,7 @@
         <v>ora2pg_mf_announcement</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="11" t="s">
         <v>23</v>
       </c>
@@ -5363,7 +4759,7 @@
         <v>142</v>
       </c>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H15" si="4">"sh ${sync_shell} "&amp;MID(E8,8,LEN(E8)-7)&amp;" ${dt} incr"</f>
+        <f t="shared" ref="H8" si="4">"sh ${sync_shell} "&amp;MID(E8,8,LEN(E8)-7)&amp;" ${dt} incr"</f>
         <v>sh ${sync_shell} mf_interimbulletin ${dt} incr</v>
       </c>
     </row>
@@ -5389,7 +4785,7 @@
         <v>ora2pg_mf_interimbulletin</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
@@ -5407,7 +4803,7 @@
         <v>142</v>
       </c>
       <c r="H10" s="5" t="str">
-        <f t="shared" ref="H10:H15" si="7">"sh ${sync_shell} "&amp;MID(E10,8,LEN(E10)-7)&amp;" ${dt} incr"</f>
+        <f t="shared" ref="H10" si="7">"sh ${sync_shell} "&amp;MID(E10,8,LEN(E10)-7)&amp;" ${dt} incr"</f>
         <v>sh ${sync_shell} mf_mmyieldperformance ${dt} incr</v>
       </c>
     </row>
@@ -5433,7 +4829,7 @@
         <v>ora2pg_mf_mmyieldperformance</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="11" t="s">
         <v>23</v>
       </c>
@@ -5451,7 +4847,7 @@
         <v>142</v>
       </c>
       <c r="H12" s="5" t="str">
-        <f t="shared" ref="H12:H15" si="10">"sh ${sync_shell} "&amp;MID(E12,8,LEN(E12)-7)&amp;" ${dt} incr"</f>
+        <f t="shared" ref="H12" si="10">"sh ${sync_shell} "&amp;MID(E12,8,LEN(E12)-7)&amp;" ${dt} incr"</f>
         <v>sh ${sync_shell} mf_netvalue ${dt} incr</v>
       </c>
     </row>
@@ -5477,7 +4873,7 @@
         <v>ora2pg_mf_netvalue</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
@@ -5495,7 +4891,7 @@
         <v>142</v>
       </c>
       <c r="H14" s="5" t="str">
-        <f t="shared" ref="H14:H15" si="13">"sh ${sync_shell} "&amp;MID(E14,8,LEN(E14)-7)&amp;" ${dt} incr"</f>
+        <f t="shared" ref="H14" si="13">"sh ${sync_shell} "&amp;MID(E14,8,LEN(E14)-7)&amp;" ${dt} incr"</f>
         <v>sh ${sync_shell} mf_netvalueperformancehis ${dt} incr</v>
       </c>
     </row>
@@ -5521,7 +4917,7 @@
         <v>ora2pg_mf_netvalueperformancehis</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
@@ -5565,7 +4961,7 @@
         <v>ora2pg_mf_assetallocation</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="11" t="s">
         <v>23</v>
       </c>
@@ -5609,7 +5005,7 @@
         <v>ora2pg_mf_balancesheetnew</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="11" t="s">
         <v>23</v>
       </c>
@@ -5653,7 +5049,7 @@
         <v>ora2pg_mf_bondportifoliodetail</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
@@ -5697,7 +5093,7 @@
         <v>ora2pg_mf_dividend</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="11" t="s">
         <v>23</v>
       </c>
@@ -5741,7 +5137,7 @@
         <v>ora2pg_mf_fundarchives</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="11" t="s">
         <v>23</v>
       </c>
@@ -5785,7 +5181,7 @@
         <v>ora2pg_mf_fundarchivesattach</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="11" t="s">
         <v>23</v>
       </c>
@@ -5829,7 +5225,7 @@
         <v>ora2pg_mf_fundmanagernew</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="11" t="s">
         <v>23</v>
       </c>
@@ -5873,7 +5269,7 @@
         <v>ora2pg_mf_fundportifoliodetail</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="11" t="s">
         <v>23</v>
       </c>
@@ -5917,7 +5313,7 @@
         <v>ora2pg_mf_incomestatementnew</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" s="11" t="s">
         <v>23</v>
       </c>
@@ -5961,7 +5357,7 @@
         <v>ora2pg_mf_interimbulletin_se</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" s="11" t="s">
         <v>23</v>
       </c>
@@ -6005,7 +5401,7 @@
         <v>ora2pg_mf_investadvisoroutline</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="11" t="s">
         <v>23</v>
       </c>
@@ -6049,7 +5445,7 @@
         <v>ora2pg_mf_investindustry</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" s="11" t="s">
         <v>23</v>
       </c>
@@ -6093,7 +5489,7 @@
         <v>ora2pg_mf_issueandlisting</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" s="11" t="s">
         <v>23</v>
       </c>
@@ -6137,7 +5533,7 @@
         <v>ora2pg_mf_keystockportfolio</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" s="11" t="s">
         <v>23</v>
       </c>
@@ -6181,7 +5577,7 @@
         <v>ora2pg_mf_mainfinancialindex</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" s="11" t="s">
         <v>23</v>
       </c>
@@ -6225,7 +5621,7 @@
         <v>ora2pg_mf_netvalueperformance</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" s="11" t="s">
         <v>23</v>
       </c>
@@ -6269,7 +5665,7 @@
         <v>ora2pg_mf_qdiiassetallocation</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="11" t="s">
         <v>23</v>
       </c>
@@ -6313,7 +5709,7 @@
         <v>ora2pg_mf_qdiiportfoliochange</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" s="11" t="s">
         <v>23</v>
       </c>
@@ -6357,7 +5753,7 @@
         <v>ora2pg_mf_qdiiportfoliodetail</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="11" t="s">
         <v>23</v>
       </c>
@@ -6401,7 +5797,7 @@
         <v>ora2pg_mf_qdiiportfolioindustry</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" s="11" t="s">
         <v>23</v>
       </c>
@@ -6445,7 +5841,7 @@
         <v>ora2pg_mf_stockportfoliochange</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" s="11" t="s">
         <v>23</v>
       </c>
@@ -6489,7 +5885,7 @@
         <v>ora2pg_mf_stockportfoliodetail</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" s="11" t="s">
         <v>23</v>
       </c>
@@ -6533,7 +5929,7 @@
         <v>ora2pg_mf_trusteeoutline</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:9">
       <c r="A62" s="11" t="s">
         <v>23</v>
       </c>
@@ -6577,7 +5973,7 @@
         <v>ora2pg_secumain</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:9">
       <c r="A64" s="11" t="s">
         <v>23</v>
       </c>
@@ -6621,7 +6017,7 @@
         <v>ora2pg_mf_chargeratenew</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:9">
       <c r="A66" s="11" t="s">
         <v>23</v>
       </c>
@@ -6642,7 +6038,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_JYDB_DELETEREC ${dt}</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:9">
       <c r="A67" s="11" t="s">
         <v>23</v>
       </c>
@@ -6661,7 +6057,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_CT_SYSTEMCONST ${dt}</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:9">
       <c r="A68" s="11" t="s">
         <v>23</v>
       </c>
@@ -6680,7 +6076,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_ANNOUNCEMENT ${dt}</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:9">
       <c r="A69" s="11" t="s">
         <v>23</v>
       </c>
@@ -6699,7 +6095,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_ASSETALLOCATION ${dt}</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:9">
       <c r="A70" s="11" t="s">
         <v>23</v>
       </c>
@@ -6718,7 +6114,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_BALANCESHEETNEW ${dt}</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:9">
       <c r="A71" s="11" t="s">
         <v>23</v>
       </c>
@@ -6737,7 +6133,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_BONDPORTIFOLIODETAIL ${dt}</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:9">
       <c r="A72" s="11" t="s">
         <v>23</v>
       </c>
@@ -6756,7 +6152,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_DIVIDEND ${dt}</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:9">
       <c r="A73" s="11" t="s">
         <v>23</v>
       </c>
@@ -6775,7 +6171,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_FUNDARCHIVES ${dt}</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:9">
       <c r="A74" s="11" t="s">
         <v>23</v>
       </c>
@@ -6794,7 +6190,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_FUNDARCHIVESATTACH ${dt}</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:9">
       <c r="A75" s="11" t="s">
         <v>23</v>
       </c>
@@ -6813,7 +6209,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_FUNDMANAGERNEW ${dt}</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:9">
       <c r="A76" s="11" t="s">
         <v>23</v>
       </c>
@@ -6832,7 +6228,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_FUNDPORTIFOLIODETAIL ${dt}</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:9">
       <c r="A77" s="11" t="s">
         <v>23</v>
       </c>
@@ -6851,7 +6247,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_INCOMESTATEMENTNEW ${dt}</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9">
       <c r="A78" s="11" t="s">
         <v>23</v>
       </c>
@@ -6870,7 +6266,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_INTERIMBULLETIN ${dt}</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9">
       <c r="A79" s="11" t="s">
         <v>23</v>
       </c>
@@ -6889,7 +6285,7 @@
         <v>sh ${check_script} ora2pg ORA2PG_MF_INTERIMBULLETIN_SE ${dt}</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9">
       <c r="A80" s="11" t="s">
         <v>23</v>
       </c>
@@ -7233,7 +6629,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:9">
       <c r="A98" s="11" t="s">
         <v>23</v>
       </c>
@@ -7298,30 +6694,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="31.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="25.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="9.83333333333333" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="57" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
@@ -7355,7 +6750,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
         <v>25</v>
       </c>
@@ -7400,7 +6795,7 @@
         <v>app2pg_bus_manager</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
@@ -7411,14 +6806,14 @@
         <v>186</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E37" si="0">LOWER(B4)</f>
+        <f t="shared" ref="E4" si="0">LOWER(B4)</f>
         <v>app2pg_prod_fund_info</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H4" s="5" t="str">
-        <f t="shared" ref="H4:H37" si="1">"sh ${sync_shell} "&amp;MID(E4,8,LEN(E4)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H4" si="1">"sh ${sync_shell} "&amp;MID(E4,8,LEN(E4)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} prod_fund_info ${dt}</v>
       </c>
     </row>
@@ -7431,7 +6826,7 @@
       </c>
       <c r="D5" s="10"/>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E37" si="2">LOWER(B5)&amp;"_done"</f>
+        <f t="shared" ref="E5" si="2">LOWER(B5)&amp;"_done"</f>
         <v>app2pg_prod_fund_info_done</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -7441,11 +6836,11 @@
         <v>187</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5:I37" si="3">LOWER(B5)</f>
+        <f t="shared" ref="I5" si="3">LOWER(B5)</f>
         <v>app2pg_prod_fund_info</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
         <v>25</v>
       </c>
@@ -7456,14 +6851,14 @@
         <v>186</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6:E37" si="4">LOWER(B6)</f>
+        <f t="shared" ref="E6" si="4">LOWER(B6)</f>
         <v>app2pg_sale_behavior_log</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H6" s="5" t="str">
-        <f t="shared" ref="H6:H37" si="5">"sh ${sync_shell} "&amp;MID(E6,8,LEN(E6)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H6" si="5">"sh ${sync_shell} "&amp;MID(E6,8,LEN(E6)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_behavior_log ${dt}</v>
       </c>
     </row>
@@ -7476,7 +6871,7 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E37" si="6">LOWER(B7)&amp;"_done"</f>
+        <f t="shared" ref="E7" si="6">LOWER(B7)&amp;"_done"</f>
         <v>app2pg_sale_behavior_log_done</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -7486,11 +6881,11 @@
         <v>187</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7:I37" si="7">LOWER(B7)</f>
+        <f t="shared" ref="I7" si="7">LOWER(B7)</f>
         <v>app2pg_sale_behavior_log</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
@@ -7501,14 +6896,14 @@
         <v>186</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" ref="E8:E37" si="8">LOWER(B8)</f>
+        <f t="shared" ref="E8" si="8">LOWER(B8)</f>
         <v>app2pg_sale_customer</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H37" si="9">"sh ${sync_shell} "&amp;MID(E8,8,LEN(E8)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H8" si="9">"sh ${sync_shell} "&amp;MID(E8,8,LEN(E8)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_customer ${dt}</v>
       </c>
     </row>
@@ -7521,7 +6916,7 @@
       </c>
       <c r="D9" s="10"/>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:E37" si="10">LOWER(B9)&amp;"_done"</f>
+        <f t="shared" ref="E9" si="10">LOWER(B9)&amp;"_done"</f>
         <v>app2pg_sale_customer_done</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -7531,11 +6926,11 @@
         <v>187</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9:I37" si="11">LOWER(B9)</f>
+        <f t="shared" ref="I9" si="11">LOWER(B9)</f>
         <v>app2pg_sale_customer</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
@@ -7546,14 +6941,14 @@
         <v>186</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ref="E10:E37" si="12">LOWER(B10)</f>
+        <f t="shared" ref="E10" si="12">LOWER(B10)</f>
         <v>app2pg_sale_fixallot</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H10" s="5" t="str">
-        <f t="shared" ref="H10:H37" si="13">"sh ${sync_shell} "&amp;MID(E10,8,LEN(E10)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H10" si="13">"sh ${sync_shell} "&amp;MID(E10,8,LEN(E10)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_fixallot ${dt}</v>
       </c>
     </row>
@@ -7566,7 +6961,7 @@
       </c>
       <c r="D11" s="10"/>
       <c r="E11" t="str">
-        <f t="shared" ref="E11:E37" si="14">LOWER(B11)&amp;"_done"</f>
+        <f t="shared" ref="E11" si="14">LOWER(B11)&amp;"_done"</f>
         <v>app2pg_sale_fixallot_done</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -7576,11 +6971,11 @@
         <v>187</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11:I37" si="15">LOWER(B11)</f>
+        <f t="shared" ref="I11" si="15">LOWER(B11)</f>
         <v>app2pg_sale_fixallot</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -7591,14 +6986,14 @@
         <v>186</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" ref="E12:E37" si="16">LOWER(B12)</f>
+        <f t="shared" ref="E12" si="16">LOWER(B12)</f>
         <v>app2pg_sale_fixallot_request</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H12" s="5" t="str">
-        <f t="shared" ref="H12:H37" si="17">"sh ${sync_shell} "&amp;MID(E12,8,LEN(E12)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H12" si="17">"sh ${sync_shell} "&amp;MID(E12,8,LEN(E12)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_fixallot_request ${dt}</v>
       </c>
     </row>
@@ -7611,7 +7006,7 @@
       </c>
       <c r="D13" s="10"/>
       <c r="E13" t="str">
-        <f t="shared" ref="E13:E37" si="18">LOWER(B13)&amp;"_done"</f>
+        <f t="shared" ref="E13" si="18">LOWER(B13)&amp;"_done"</f>
         <v>app2pg_sale_fixallot_request_done</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -7621,11 +7016,11 @@
         <v>187</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I37" si="19">LOWER(B13)</f>
+        <f t="shared" ref="I13" si="19">LOWER(B13)</f>
         <v>app2pg_sale_fixallot_request</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="9" t="s">
         <v>25</v>
       </c>
@@ -7636,14 +7031,14 @@
         <v>186</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ref="E14:E37" si="20">LOWER(B14)</f>
+        <f t="shared" ref="E14" si="20">LOWER(B14)</f>
         <v>app2pg_sale_invite</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H14" s="5" t="str">
-        <f t="shared" ref="H14:H37" si="21">"sh ${sync_shell} "&amp;MID(E14,8,LEN(E14)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H14" si="21">"sh ${sync_shell} "&amp;MID(E14,8,LEN(E14)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_invite ${dt}</v>
       </c>
     </row>
@@ -7656,7 +7051,7 @@
       </c>
       <c r="D15" s="10"/>
       <c r="E15" t="str">
-        <f t="shared" ref="E15:E37" si="22">LOWER(B15)&amp;"_done"</f>
+        <f t="shared" ref="E15" si="22">LOWER(B15)&amp;"_done"</f>
         <v>app2pg_sale_invite_done</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -7666,11 +7061,11 @@
         <v>187</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15:I37" si="23">LOWER(B15)</f>
+        <f t="shared" ref="I15" si="23">LOWER(B15)</f>
         <v>app2pg_sale_invite</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
@@ -7681,14 +7076,14 @@
         <v>186</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ref="E16:E37" si="24">LOWER(B16)</f>
+        <f t="shared" ref="E16" si="24">LOWER(B16)</f>
         <v>app2pg_sale_order</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H16" s="5" t="str">
-        <f t="shared" ref="H16:H37" si="25">"sh ${sync_shell} "&amp;MID(E16,8,LEN(E16)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H16" si="25">"sh ${sync_shell} "&amp;MID(E16,8,LEN(E16)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_order ${dt}</v>
       </c>
     </row>
@@ -7701,7 +7096,7 @@
       </c>
       <c r="D17" s="10"/>
       <c r="E17" t="str">
-        <f t="shared" ref="E17:E37" si="26">LOWER(B17)&amp;"_done"</f>
+        <f t="shared" ref="E17" si="26">LOWER(B17)&amp;"_done"</f>
         <v>app2pg_sale_order_done</v>
       </c>
       <c r="G17" s="5" t="s">
@@ -7711,11 +7106,11 @@
         <v>187</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" ref="I17:I37" si="27">LOWER(B17)</f>
+        <f t="shared" ref="I17" si="27">LOWER(B17)</f>
         <v>app2pg_sale_order</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="9" t="s">
         <v>25</v>
       </c>
@@ -7726,14 +7121,14 @@
         <v>186</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" ref="E18:E37" si="28">LOWER(B18)</f>
+        <f t="shared" ref="E18" si="28">LOWER(B18)</f>
         <v>app2pg_sale_user_position</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H18" s="5" t="str">
-        <f t="shared" ref="H18:H37" si="29">"sh ${sync_shell} "&amp;MID(E18,8,LEN(E18)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H18" si="29">"sh ${sync_shell} "&amp;MID(E18,8,LEN(E18)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sale_user_position ${dt}</v>
       </c>
     </row>
@@ -7746,7 +7141,7 @@
       </c>
       <c r="D19" s="10"/>
       <c r="E19" t="str">
-        <f t="shared" ref="E19:E37" si="30">LOWER(B19)&amp;"_done"</f>
+        <f t="shared" ref="E19" si="30">LOWER(B19)&amp;"_done"</f>
         <v>app2pg_sale_user_position_done</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -7756,11 +7151,11 @@
         <v>187</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" ref="I19:I37" si="31">LOWER(B19)</f>
+        <f t="shared" ref="I19" si="31">LOWER(B19)</f>
         <v>app2pg_sale_user_position</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
@@ -7771,14 +7166,14 @@
         <v>186</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" ref="E20:E37" si="32">LOWER(B20)</f>
+        <f t="shared" ref="E20" si="32">LOWER(B20)</f>
         <v>app2pg_sys_channel_pop</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H20" s="5" t="str">
-        <f t="shared" ref="H20:H37" si="33">"sh ${sync_shell} "&amp;MID(E20,8,LEN(E20)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H20" si="33">"sh ${sync_shell} "&amp;MID(E20,8,LEN(E20)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_channel_pop ${dt}</v>
       </c>
     </row>
@@ -7791,7 +7186,7 @@
       </c>
       <c r="D21" s="10"/>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E37" si="34">LOWER(B21)&amp;"_done"</f>
+        <f t="shared" ref="E21" si="34">LOWER(B21)&amp;"_done"</f>
         <v>app2pg_sys_channel_pop_done</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -7801,11 +7196,11 @@
         <v>187</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" ref="I21:I37" si="35">LOWER(B21)</f>
+        <f t="shared" ref="I21" si="35">LOWER(B21)</f>
         <v>app2pg_sys_channel_pop</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
@@ -7816,14 +7211,14 @@
         <v>186</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" ref="E22:E37" si="36">LOWER(B22)</f>
+        <f t="shared" ref="E22" si="36">LOWER(B22)</f>
         <v>app2pg_sys_cust_bus</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H22" s="5" t="str">
-        <f t="shared" ref="H22:H37" si="37">"sh ${sync_shell} "&amp;MID(E22,8,LEN(E22)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H22" si="37">"sh ${sync_shell} "&amp;MID(E22,8,LEN(E22)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_cust_bus ${dt}</v>
       </c>
     </row>
@@ -7836,7 +7231,7 @@
       </c>
       <c r="D23" s="10"/>
       <c r="E23" t="str">
-        <f t="shared" ref="E23:E37" si="38">LOWER(B23)&amp;"_done"</f>
+        <f t="shared" ref="E23" si="38">LOWER(B23)&amp;"_done"</f>
         <v>app2pg_sys_cust_bus_done</v>
       </c>
       <c r="G23" s="5" t="s">
@@ -7846,11 +7241,11 @@
         <v>187</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" ref="I23:I37" si="39">LOWER(B23)</f>
+        <f t="shared" ref="I23" si="39">LOWER(B23)</f>
         <v>app2pg_sys_cust_bus</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
@@ -7861,14 +7256,14 @@
         <v>186</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" ref="E24:E37" si="40">LOWER(B24)</f>
+        <f t="shared" ref="E24" si="40">LOWER(B24)</f>
         <v>app2pg_sys_dict_data</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H24" s="5" t="str">
-        <f t="shared" ref="H24:H37" si="41">"sh ${sync_shell} "&amp;MID(E24,8,LEN(E24)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H24" si="41">"sh ${sync_shell} "&amp;MID(E24,8,LEN(E24)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_dict_data ${dt}</v>
       </c>
     </row>
@@ -7881,7 +7276,7 @@
       </c>
       <c r="D25" s="10"/>
       <c r="E25" t="str">
-        <f t="shared" ref="E25:E37" si="42">LOWER(B25)&amp;"_done"</f>
+        <f t="shared" ref="E25" si="42">LOWER(B25)&amp;"_done"</f>
         <v>app2pg_sys_dict_data_done</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -7891,11 +7286,11 @@
         <v>187</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" ref="I25:I37" si="43">LOWER(B25)</f>
+        <f t="shared" ref="I25" si="43">LOWER(B25)</f>
         <v>app2pg_sys_dict_data</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="9" t="s">
         <v>25</v>
       </c>
@@ -7906,14 +7301,14 @@
         <v>186</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" ref="E26:E37" si="44">LOWER(B26)</f>
+        <f t="shared" ref="E26" si="44">LOWER(B26)</f>
         <v>app2pg_sys_manage_business</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H26" s="5" t="str">
-        <f t="shared" ref="H26:H37" si="45">"sh ${sync_shell} "&amp;MID(E26,8,LEN(E26)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H26" si="45">"sh ${sync_shell} "&amp;MID(E26,8,LEN(E26)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_manage_business ${dt}</v>
       </c>
     </row>
@@ -7926,7 +7321,7 @@
       </c>
       <c r="D27" s="10"/>
       <c r="E27" t="str">
-        <f t="shared" ref="E27:E37" si="46">LOWER(B27)&amp;"_done"</f>
+        <f t="shared" ref="E27" si="46">LOWER(B27)&amp;"_done"</f>
         <v>app2pg_sys_manage_business_done</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -7936,11 +7331,11 @@
         <v>187</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" ref="I27:I37" si="47">LOWER(B27)</f>
+        <f t="shared" ref="I27" si="47">LOWER(B27)</f>
         <v>app2pg_sys_manage_business</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
@@ -7951,14 +7346,14 @@
         <v>186</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" ref="E28:E37" si="48">LOWER(B28)</f>
+        <f t="shared" ref="E28" si="48">LOWER(B28)</f>
         <v>app2pg_sys_region</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H28" s="5" t="str">
-        <f t="shared" ref="H28:H37" si="49">"sh ${sync_shell} "&amp;MID(E28,8,LEN(E28)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H28" si="49">"sh ${sync_shell} "&amp;MID(E28,8,LEN(E28)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_region ${dt}</v>
       </c>
     </row>
@@ -7971,7 +7366,7 @@
       </c>
       <c r="D29" s="10"/>
       <c r="E29" t="str">
-        <f t="shared" ref="E29:E37" si="50">LOWER(B29)&amp;"_done"</f>
+        <f t="shared" ref="E29" si="50">LOWER(B29)&amp;"_done"</f>
         <v>app2pg_sys_region_done</v>
       </c>
       <c r="G29" s="5" t="s">
@@ -7981,11 +7376,11 @@
         <v>187</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" ref="I29:I37" si="51">LOWER(B29)</f>
+        <f t="shared" ref="I29" si="51">LOWER(B29)</f>
         <v>app2pg_sys_region</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="9" t="s">
         <v>25</v>
       </c>
@@ -7996,14 +7391,14 @@
         <v>186</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" ref="E30:E37" si="52">LOWER(B30)</f>
+        <f t="shared" ref="E30" si="52">LOWER(B30)</f>
         <v>app2pg_sys_region_business</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H30" s="5" t="str">
-        <f t="shared" ref="H30:H37" si="53">"sh ${sync_shell} "&amp;MID(E30,8,LEN(E30)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H30" si="53">"sh ${sync_shell} "&amp;MID(E30,8,LEN(E30)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_region_business ${dt}</v>
       </c>
     </row>
@@ -8016,7 +7411,7 @@
       </c>
       <c r="D31" s="10"/>
       <c r="E31" t="str">
-        <f t="shared" ref="E31:E37" si="54">LOWER(B31)&amp;"_done"</f>
+        <f t="shared" ref="E31" si="54">LOWER(B31)&amp;"_done"</f>
         <v>app2pg_sys_region_business_done</v>
       </c>
       <c r="G31" s="5" t="s">
@@ -8026,11 +7421,11 @@
         <v>187</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" ref="I31:I37" si="55">LOWER(B31)</f>
+        <f t="shared" ref="I31" si="55">LOWER(B31)</f>
         <v>app2pg_sys_region_business</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="9" t="s">
         <v>25</v>
       </c>
@@ -8041,14 +7436,14 @@
         <v>186</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" ref="E32:E37" si="56">LOWER(B32)</f>
+        <f t="shared" ref="E32" si="56">LOWER(B32)</f>
         <v>app2pg_sys_team</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H32" s="5" t="str">
-        <f t="shared" ref="H32:H37" si="57">"sh ${sync_shell} "&amp;MID(E32,8,LEN(E32)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H32" si="57">"sh ${sync_shell} "&amp;MID(E32,8,LEN(E32)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_team ${dt}</v>
       </c>
     </row>
@@ -8061,7 +7456,7 @@
       </c>
       <c r="D33" s="10"/>
       <c r="E33" t="str">
-        <f t="shared" ref="E33:E37" si="58">LOWER(B33)&amp;"_done"</f>
+        <f t="shared" ref="E33" si="58">LOWER(B33)&amp;"_done"</f>
         <v>app2pg_sys_team_done</v>
       </c>
       <c r="G33" s="5" t="s">
@@ -8071,11 +7466,11 @@
         <v>187</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" ref="I33:I37" si="59">LOWER(B33)</f>
+        <f t="shared" ref="I33" si="59">LOWER(B33)</f>
         <v>app2pg_sys_team</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" s="9" t="s">
         <v>25</v>
       </c>
@@ -8086,14 +7481,14 @@
         <v>186</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ref="E34:E37" si="60">LOWER(B34)</f>
+        <f t="shared" ref="E34" si="60">LOWER(B34)</f>
         <v>app2pg_sys_team_business</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H34" s="5" t="str">
-        <f t="shared" ref="H34:H37" si="61">"sh ${sync_shell} "&amp;MID(E34,8,LEN(E34)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H34" si="61">"sh ${sync_shell} "&amp;MID(E34,8,LEN(E34)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_team_business ${dt}</v>
       </c>
     </row>
@@ -8106,7 +7501,7 @@
       </c>
       <c r="D35" s="10"/>
       <c r="E35" t="str">
-        <f t="shared" ref="E35:E37" si="62">LOWER(B35)&amp;"_done"</f>
+        <f t="shared" ref="E35" si="62">LOWER(B35)&amp;"_done"</f>
         <v>app2pg_sys_team_business_done</v>
       </c>
       <c r="G35" s="5" t="s">
@@ -8116,11 +7511,11 @@
         <v>187</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" ref="I35:I37" si="63">LOWER(B35)</f>
+        <f t="shared" ref="I35" si="63">LOWER(B35)</f>
         <v>app2pg_sys_team_business</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" s="9" t="s">
         <v>25</v>
       </c>
@@ -8131,14 +7526,14 @@
         <v>186</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" ref="E36:E37" si="64">LOWER(B36)</f>
+        <f t="shared" ref="E36" si="64">LOWER(B36)</f>
         <v>app2pg_sys_team_manager</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H36" s="5" t="str">
-        <f t="shared" ref="H36:H37" si="65">"sh ${sync_shell} "&amp;MID(E36,8,LEN(E36)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H36" si="65">"sh ${sync_shell} "&amp;MID(E36,8,LEN(E36)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_team_manager ${dt}</v>
       </c>
     </row>
@@ -8165,7 +7560,7 @@
         <v>app2pg_sys_team_manager</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="9" t="s">
         <v>25</v>
       </c>
@@ -8176,14 +7571,14 @@
         <v>186</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" ref="E38:E39" si="68">LOWER(B38)</f>
+        <f t="shared" ref="E38" si="68">LOWER(B38)</f>
         <v>app2pg_sys_user</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>142</v>
       </c>
       <c r="H38" s="5" t="str">
-        <f t="shared" ref="H38:H39" si="69">"sh ${sync_shell} "&amp;MID(E38,8,LEN(E38)-7)&amp;" ${dt}"</f>
+        <f t="shared" ref="H38" si="69">"sh ${sync_shell} "&amp;MID(E38,8,LEN(E38)-7)&amp;" ${dt}"</f>
         <v>sh ${sync_shell} sys_user ${dt}</v>
       </c>
     </row>
@@ -8210,7 +7605,7 @@
         <v>app2pg_sys_user</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" s="9" t="s">
         <v>25</v>
       </c>
@@ -8231,7 +7626,7 @@
         <v>sh ${check_script} app2pg APP2PG_BUS_MANAGER $dt</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" s="9" t="s">
         <v>25</v>
       </c>
@@ -8249,7 +7644,7 @@
         <v>sh ${check_script} app2pg APP2PG_PROD_FUND_INFO $dt</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" s="9" t="s">
         <v>25</v>
       </c>
@@ -8267,7 +7662,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_BEHAVIOR_LOG $dt</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="A43" s="9" t="s">
         <v>25</v>
       </c>
@@ -8285,7 +7680,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_CUSTOMER $dt</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" s="9" t="s">
         <v>25</v>
       </c>
@@ -8303,7 +7698,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_FIXALLOT $dt</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="A45" s="9" t="s">
         <v>25</v>
       </c>
@@ -8321,7 +7716,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_FIXALLOT_REQUEST $dt</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" s="9" t="s">
         <v>25</v>
       </c>
@@ -8339,7 +7734,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_INVITE $dt</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9">
       <c r="A47" s="9" t="s">
         <v>25</v>
       </c>
@@ -8357,7 +7752,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_ORDER $dt</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" s="9" t="s">
         <v>25</v>
       </c>
@@ -8375,7 +7770,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_USER_POSITION $dt</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" s="9" t="s">
         <v>25</v>
       </c>
@@ -8393,7 +7788,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_CHANNEL_POP $dt</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="9" t="s">
         <v>25</v>
       </c>
@@ -8411,7 +7806,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_CUST_BUS $dt</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" s="9" t="s">
         <v>25</v>
       </c>
@@ -8429,7 +7824,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_DICT_DATA $dt</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" s="9" t="s">
         <v>25</v>
       </c>
@@ -8447,7 +7842,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_MANAGE_BUSINESS $dt</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" s="9" t="s">
         <v>25</v>
       </c>
@@ -8465,7 +7860,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_REGION $dt</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="9" t="s">
         <v>25</v>
       </c>
@@ -8483,7 +7878,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_REGION_BUSINESS $dt</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:9">
       <c r="A55" s="9" t="s">
         <v>25</v>
       </c>
@@ -8501,7 +7896,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_TEAM $dt</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" s="9" t="s">
         <v>25</v>
       </c>
@@ -8519,7 +7914,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_TEAM_BUSINESS $dt</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:9">
       <c r="A57" s="9" t="s">
         <v>25</v>
       </c>
@@ -8537,7 +7932,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_TEAM_MANAGER $dt</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" s="9" t="s">
         <v>25</v>
       </c>
@@ -8576,35 +7971,33 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K180"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="41.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="13.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="41.5" customWidth="1"/>
-    <col min="6" max="6" width="12.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="67.1666666666667" customWidth="1"/>
-    <col min="9" max="9" width="20.8333333333333" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="67.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -8633,7 +8026,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -8655,7 +8048,7 @@
       </c>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -8674,7 +8067,7 @@
       </c>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -8694,7 +8087,7 @@
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -8740,7 +8133,7 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -8762,7 +8155,7 @@
       </c>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -8782,7 +8175,7 @@
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -8802,7 +8195,7 @@
       </c>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -8822,7 +8215,7 @@
       </c>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -8842,7 +8235,7 @@
       </c>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -8862,7 +8255,7 @@
       </c>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -8882,7 +8275,7 @@
       </c>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -8902,7 +8295,7 @@
       </c>
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -8925,7 +8318,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -12288,33 +11681,32 @@
       <c r="C180" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="29.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="9.83333333333333" customWidth="1"/>
-    <col min="8" max="8" width="59.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="12.8333333333333" customWidth="1"/>
-    <col min="11" max="11" width="19.8333333333333" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="59.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12346,7 +11738,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -12413,7 +11805,7 @@
         <v>bi_user_behavior_info</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -12434,7 +11826,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_USER_POSITION $dt</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -12452,7 +11844,7 @@
         <v>sh ${check_script} ods ODS_GIL_FUND_BASE_INFO $dt</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -12516,7 +11908,7 @@
         <v>bi_user_holding_info</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -12537,7 +11929,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_CUSTOMER $dt</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -12555,7 +11947,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_CUST_BUS $dt</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -12573,7 +11965,7 @@
         <v>sh ${check_script} app2pg APP2PG_BUS_MANAGER $dt</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -12591,7 +11983,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_TEAM_MANAGER $dt</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -12609,7 +12001,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_TEAM $dt</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -12627,7 +12019,7 @@
         <v>sh ${check_script} app2pg APP2PG_SYS_REGION $dt</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -12645,7 +12037,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_INVITE $dt</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -12663,7 +12055,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_BEHAVIOR_LOG $dt</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -12681,7 +12073,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_ORDER $dt</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -12699,7 +12091,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_FIXALLOT_REQUEST $dt</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -12763,7 +12155,7 @@
         <v>bi_user_info</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -12784,7 +12176,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_ORDER $dt</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -12802,7 +12194,7 @@
         <v>sh ${check_script} app2pg APP2PG_SALE_FIXALLOT_REQUEST $dt</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -12866,7 +12258,7 @@
         <v>bi_user_order_info</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -12887,7 +12279,7 @@
         <v>sh ${check_script} app2pg APP2PG_PROD_FUND_INFO $dt</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -12905,7 +12297,7 @@
         <v>sh ${check_script} bi BI_USER_ORDER_INFO $dt</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -12923,7 +12315,7 @@
         <v>sh ${check_script} bi BI_USER_HOLDING_INFO $dt</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -12987,7 +12379,7 @@
         <v>bi_user_prd_ord_hold_info</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
@@ -13008,7 +12400,7 @@
         <v>sh ${check_script} bi BI_USER_INFO $dt</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
@@ -13072,7 +12464,7 @@
         <v>rpt_behavior_trend_year</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
         <v>27</v>
       </c>
@@ -13093,7 +12485,7 @@
         <v>sh ${check_script} bi BI_USER_INFO $dt</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
         <v>27</v>
       </c>
@@ -13111,7 +12503,7 @@
         <v>sh ${check_script} bi BI_USER_ORDER_INFO $dt</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
@@ -13175,7 +12567,7 @@
         <v>rpt_oper_data</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
         <v>27</v>
       </c>
@@ -13196,7 +12588,7 @@
         <v>sh ${check_script} bi BI_USER_INFO $dt</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
         <v>27</v>
       </c>
@@ -13214,7 +12606,7 @@
         <v>sh ${check_script} bi BI_USER_HOLDING_INFO $dt</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
         <v>27</v>
       </c>
@@ -13278,7 +12670,7 @@
         <v>rpt_reg_source</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
         <v>27</v>
       </c>
@@ -13299,7 +12691,7 @@
         <v>sh ${check_script} bi BI_USER_INFO $dt</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" s="2" t="s">
         <v>27</v>
       </c>
@@ -13317,7 +12709,7 @@
         <v>sh ${check_script} bi BI_USER_ORDER_INFO $dt</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="2" t="s">
         <v>27</v>
       </c>
@@ -13377,7 +12769,7 @@
         <v>rpt_sale_busi_data</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" s="2" t="s">
         <v>27</v>
       </c>
@@ -13399,7 +12791,7 @@
         <v>sh ${check_script} bi BI_USER_BEHAVIOR_INFO $dt</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="2" t="s">
         <v>27</v>
       </c>
@@ -13417,7 +12809,7 @@
         <v>sh ${check_script} bi BI_USER_HOLDING_INFO $dt</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:9">
       <c r="A55" s="2" t="s">
         <v>27</v>
       </c>
@@ -13435,7 +12827,7 @@
         <v>sh ${check_script} bi BI_USER_INFO $dt</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -13453,7 +12845,7 @@
         <v>sh ${check_script} bi BI_USER_ORDER_INFO $dt</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:9">
       <c r="A57" s="2" t="s">
         <v>27</v>
       </c>
@@ -13471,7 +12863,7 @@
         <v>sh ${check_script} bi BI_USER_PRD_ORD_HOLD_INFO $dt</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" s="2" t="s">
         <v>27</v>
       </c>
@@ -13489,7 +12881,7 @@
         <v>sh ${check_script} bi RPT_BEHAVIOR_TREND_YEAR $dt</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:9">
       <c r="A59" s="2" t="s">
         <v>27</v>
       </c>
@@ -13507,7 +12899,7 @@
         <v>sh ${check_script} bi RPT_OPER_DATA $dt</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" s="2" t="s">
         <v>27</v>
       </c>
@@ -13525,7 +12917,7 @@
         <v>sh ${check_script} bi RPT_REG_SOURCE $dt</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:9">
       <c r="A61" s="2" t="s">
         <v>27</v>
       </c>
@@ -13564,32 +12956,31 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="20.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="36.1666666666667" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="9.83333333333333" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="69" customWidth="1"/>
-    <col min="9" max="9" width="12.8333333333333" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -13621,7 +13012,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -13685,7 +13076,7 @@
         <v>assetallocation</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -13749,7 +13140,7 @@
         <v>awnstock</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -13813,7 +13204,7 @@
         <v>bondportifolio</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -13877,7 +13268,7 @@
         <v>fundannview</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -13941,7 +13332,7 @@
         <v>fundbal</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -14005,7 +13396,7 @@
         <v>fundbase</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -14069,7 +13460,7 @@
         <v>fundcomp</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -14133,7 +13524,7 @@
         <v>fundcompmgr</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -14197,7 +13588,7 @@
         <v>funddiv</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -14261,7 +13652,7 @@
         <v>fundinc</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
         <v>26</v>
       </c>
@@ -14325,7 +13716,7 @@
         <v>fundmainfin</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
@@ -14361,7 +13752,7 @@
       </c>
       <c r="H36" s="2" t="str">
         <f>"sh ${|manager_script} ${dt} "&amp;LOWER(B36)&amp;" "</f>
-        <v>sh ${|manager_script} ${dt} fundmanager </v>
+        <v xml:space="preserve">sh ${|manager_script} ${dt} fundmanager </v>
       </c>
       <c r="I36" t="str">
         <f t="shared" ref="I36:I37" si="21">E35</f>
@@ -14389,7 +13780,7 @@
         <v>fundmanager</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
         <v>26</v>
       </c>
@@ -14453,7 +13844,7 @@
         <v>fundmoney</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
         <v>26</v>
       </c>
@@ -14517,7 +13908,7 @@
         <v>fundnav_newest</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
         <v>26</v>
       </c>
@@ -14581,7 +13972,7 @@
         <v>fundportifolio</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9">
       <c r="A47" s="2" t="s">
         <v>26</v>
       </c>
@@ -14645,7 +14036,7 @@
         <v>industryportifolio</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="2" t="s">
         <v>26</v>
       </c>
@@ -14709,7 +14100,7 @@
         <v>secuchange</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" s="2" t="s">
         <v>26</v>
       </c>
@@ -14773,7 +14164,7 @@
         <v>stockportifolio</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
         <v>26</v>
       </c>
@@ -14794,7 +14185,7 @@
         <v>sh ${check_script} pg2mongo ASSETALLOCATION $dt</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:9">
       <c r="A57" s="2" t="s">
         <v>26</v>
       </c>
@@ -14812,7 +14203,7 @@
         <v>sh ${check_script} pg2mongo AWNSTOCK $dt</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" s="2" t="s">
         <v>26</v>
       </c>
@@ -14830,7 +14221,7 @@
         <v>sh ${check_script} pg2mongo BONDPORTIFOLIO $dt</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:9">
       <c r="A59" s="2" t="s">
         <v>26</v>
       </c>
@@ -14848,7 +14239,7 @@
         <v>sh ${check_script} pg2mongo FUNDANNVIEW $dt</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
@@ -14866,7 +14257,7 @@
         <v>sh ${check_script} pg2mongo FUNDBAL $dt</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:9">
       <c r="A61" s="2" t="s">
         <v>26</v>
       </c>
@@ -14884,7 +14275,7 @@
         <v>sh ${check_script} pg2mongo FUNDBASE $dt</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:9">
       <c r="A62" s="2" t="s">
         <v>26</v>
       </c>
@@ -14902,7 +14293,7 @@
         <v>sh ${check_script} pg2mongo FUNDCOMP $dt</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:9">
       <c r="A63" s="2" t="s">
         <v>26</v>
       </c>
@@ -14920,7 +14311,7 @@
         <v>sh ${check_script} pg2mongo FUNDCOMPMGR $dt</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:9">
       <c r="A64" s="2" t="s">
         <v>26</v>
       </c>
@@ -14938,7 +14329,7 @@
         <v>sh ${check_script} pg2mongo FUNDDIV $dt</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:9">
       <c r="A65" s="2" t="s">
         <v>26</v>
       </c>
@@ -14956,7 +14347,7 @@
         <v>sh ${check_script} pg2mongo FUNDINC $dt</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:9">
       <c r="A66" s="2" t="s">
         <v>26</v>
       </c>
@@ -14974,7 +14365,7 @@
         <v>sh ${check_script} pg2mongo FUNDMAINFIN $dt</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:9">
       <c r="A67" s="2" t="s">
         <v>26</v>
       </c>
@@ -14992,7 +14383,7 @@
         <v>sh ${check_script} pg2mongo FUNDMANAGER $dt</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:9">
       <c r="A68" s="2" t="s">
         <v>26</v>
       </c>
@@ -15010,7 +14401,7 @@
         <v>sh ${check_script} pg2mongo FUNDMONEY $dt</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:9">
       <c r="A69" s="2" t="s">
         <v>26</v>
       </c>
@@ -15028,7 +14419,7 @@
         <v>sh ${check_script} pg2mongo FUNDNAV_NEWEST $dt</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:9">
       <c r="A70" s="2" t="s">
         <v>26</v>
       </c>
@@ -15046,7 +14437,7 @@
         <v>sh ${check_script} pg2mongo FUNDPORTIFOLIO $dt</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:9">
       <c r="A71" s="2" t="s">
         <v>26</v>
       </c>
@@ -15064,7 +14455,7 @@
         <v>sh ${check_script} pg2mongo INDUSTRYPORTIFOLIO $dt</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:9">
       <c r="A72" s="2" t="s">
         <v>26</v>
       </c>
@@ -15082,7 +14473,7 @@
         <v>sh ${check_script} pg2mongo SECUCHANGE $dt</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:9">
       <c r="A73" s="2" t="s">
         <v>26</v>
       </c>
@@ -15120,12 +14511,12 @@
         <v>355</v>
       </c>
     </row>
-    <row r="76" spans="4:4">
+    <row r="76" spans="1:9">
       <c r="D76" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The v1.0.0 release update
</commit_message>
<xml_diff>
--- a/docs/template.xlsx
+++ b/docs/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/PycharmProjects/azkaban_excel_yaml/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE7BB0-F9BB-0B43-868D-A94B6B84E019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BEDF4E-0A84-9349-B7E6-A0719337335C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
   <si>
     <t>Overview</t>
   </si>
@@ -327,6 +327,21 @@
     <t>check_flow_a|check_flow_b|check_flow_c|check_flow_d|check_flow_e|check_flow_f</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes:    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Only the first row will be used exclude the title row.</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -335,7 +350,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +406,20 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -523,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,6 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -883,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -988,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1053,6 +1083,14 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1116,6 +1154,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1123,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add set SLA function
</commit_message>
<xml_diff>
--- a/docs/template.xlsx
+++ b/docs/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/PycharmProjects/azkaban_excel_yaml/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA48A6-E2AF-B74D-91B9-D35387D55535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73986CE7-9726-2E46-A00D-9B3461BD2739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -26,8 +26,284 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EA1270DF-7AB1-DA4B-A95A-097CBBCC7306}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>未启用，但不能删除，仅用于生成</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>crontab</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>表达式</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E10A2847-CB1D-6149-B209-0FCF18D8A0A4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>D</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>列为</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>True</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>时，</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SLA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>才会生效</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{C5D544CF-D14C-4146-8DA0-CDE57FBFAD3A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>多个邮件地址用分号分隔</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{5E2D3036-3682-5B42-A396-AE0AEB0DABBD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>只能是该</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>FLOW</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>的所有节点中的一个，暂不支持多个</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{0C90AFBC-D4AD-414B-A248-08CA2F34C6F6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>时间格式为</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">  </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>时</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>分</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{B64ABDAA-0F6D-1D47-BA0E-1AE71A35FC25}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>是否发送邮件</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>发送邮件和结束任务至少选则一个</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{1AC2B8C1-66A2-6849-9488-9519BD3AADA6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Microsoft YaHei UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>是否结束任务</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
   <si>
     <t>Overview</t>
   </si>
@@ -77,9 +353,6 @@
   </si>
   <si>
     <t>window test env</t>
-  </si>
-  <si>
-    <t>https://192.168.31.36:18443/</t>
   </si>
   <si>
     <t>/Users/jing/jbf/jobs</t>
@@ -281,9 +554,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>su - pg -c "sh ${create_script} ora3pg ${azkaban.flow.flowid} ${dt}"</t>
-  </si>
-  <si>
     <t>su - pg -c "sh ${create_script} ora4pg ${azkaban.flow.flowid} ${dt}"</t>
   </si>
   <si>
@@ -395,6 +665,87 @@
     <t>https://github.com/JingZhang-Cherish/azkaban_excel_yaml</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>sla_enabled</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>sla_emails</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flow/job</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>rule</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>email_action</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>kill_action</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1126199037@qq.com</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>durtion(HH:MM)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:02</t>
+  </si>
+  <si>
+    <t>00:03</t>
+  </si>
+  <si>
+    <t>00:04</t>
+  </si>
+  <si>
+    <t>00:05</t>
+  </si>
+  <si>
+    <t>00:06</t>
+  </si>
+  <si>
+    <t>00:07</t>
+  </si>
+  <si>
+    <t>https://192.168.31.36:18443/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1126199037@qq.com;244612023@qq.com</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>echo bbb</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>echo bbb_done</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flowPriority=50|sync_shell=/home/pg/tools/migration/gil/sync_data.sh|</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flowPriority=50|sync_shell=/home/pg/tools/migration/gil/sync_data.sh|failure.emails=244612023@qq.com</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:02</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -403,7 +754,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,8 +833,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +857,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,7 +991,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -678,6 +1054,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -693,12 +1079,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -977,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -993,29 +1374,29 @@
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:4" ht="44" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="17"/>
-      <c r="B3" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>68</v>
+      <c r="B3" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16">
@@ -1035,10 +1416,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="23">
         <v>44463</v>
@@ -1049,10 +1430,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="23">
         <v>44469</v>
@@ -1101,7 +1482,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1131,8 +1512,8 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="25" t="s">
-        <v>16</v>
+      <c r="A2" s="32" t="s">
+        <v>82</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>13</v>
@@ -1141,10 +1522,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1166,7 +1547,7 @@
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -1174,6 +1555,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6B8E32BD-1905-7C41-BB26-21970D225511}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1194,21 +1578,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>20</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1239,80 +1623,134 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:N98"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="57.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="24" t="str">
         <f>G2&amp;" "&amp;F2&amp;" "&amp;E2&amp;" ? * *"</f>
-        <v>0 11 0 ? * *</v>
+        <v>0 16 20 ? * *</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J8" si="0">B2</f>
+        <v>FLOW_A</v>
+      </c>
+      <c r="K2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="24" t="str">
-        <f t="shared" ref="C3:C8" si="0">G3&amp;" "&amp;F3&amp;" "&amp;E3&amp;" ? * *"</f>
+        <f t="shared" ref="C3:C8" si="1">G3&amp;" "&amp;F3&amp;" "&amp;E3&amp;" ? * *"</f>
         <v>0 12 0 ? * *</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1323,16 +1761,38 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>FLOW_B</v>
+      </c>
+      <c r="K3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0 13 0 ? * *</v>
       </c>
       <c r="D4" t="b">
@@ -1347,16 +1807,38 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>FLOW_C</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0 14 0 ? * *</v>
       </c>
       <c r="D5" t="b">
@@ -1371,16 +1853,38 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>FLOW_D</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0 15 0 ? * *</v>
       </c>
       <c r="D6" t="b">
@@ -1395,16 +1899,38 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>FLOW_E</v>
+      </c>
+      <c r="K6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0 16 0 ? * *</v>
       </c>
       <c r="D7" t="b">
@@ -1419,16 +1945,38 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>FLOW_F</v>
+      </c>
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0 17 0 ? * *</v>
       </c>
       <c r="D8" t="b">
@@ -1443,36 +1991,58 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>FLOW_DONE</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="9"/>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:14">
       <c r="A10" s="9"/>
       <c r="C10" s="24"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:14">
       <c r="A11" s="9"/>
       <c r="C11" s="24"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:14">
       <c r="A12" s="9"/>
       <c r="C12" s="24"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:14">
       <c r="A13" s="9"/>
       <c r="C13" s="24"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:14">
       <c r="A14" s="9"/>
       <c r="C14" s="24"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:14">
       <c r="A15" s="9"/>
       <c r="C15" s="24"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:14">
       <c r="A16" s="7"/>
       <c r="C16" s="24"/>
     </row>
@@ -1830,14 +2400,19 @@
       <c r="C98" s="24"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D98" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D98 M2:N8 H2:H8" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"True,False"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K8" xr:uid="{D9D7053E-0D60-B545-929D-5DD0B0F84A19}">
+      <formula1>"SUCCESS,FINISH"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1845,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.83203125" defaultRowHeight="15"/>
@@ -1864,71 +2439,72 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>34</v>
+        <v>44</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="E2" t="str">
         <f>LOWER(B2)</f>
         <v>flow_a</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="5" t="str">
-        <f>"sh ${sync_shell} "&amp;E2&amp;" ${dt}"</f>
-        <v>sh ${sync_shell} flow_a ${dt}</v>
+        <f>"sleep 200"</f>
+        <v>sleep 200</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="H3" s="5" t="str">
+        <f>"sleep 1"</f>
+        <v>sleep 1</v>
       </c>
       <c r="I3" s="5" t="str">
         <f>E2</f>
@@ -1937,13 +2513,13 @@
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1">
       <c r="A4" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>34</v>
+        <v>45</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>86</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ref="E4" si="0">LOWER(B4)</f>
@@ -1951,32 +2527,31 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="5" t="str">
-        <f t="shared" ref="H4" si="1">"sh ${sync_shell} "&amp;E4&amp;" ${dt}"</f>
-        <v>sh ${sync_shell} flow_b ${dt}</v>
+        <v>31</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="11"/>
       <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>51</v>
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="I5" s="5" t="str">
         <f>E4</f>
@@ -1985,195 +2560,195 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6" si="2">LOWER(B6)</f>
+        <f t="shared" ref="E6" si="1">LOWER(B6)</f>
         <v>flow_c</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="5" t="str">
-        <f t="shared" ref="H6" si="3">"sh ${sync_shell} "&amp;E6&amp;" ${dt}"</f>
+        <f t="shared" ref="H6" si="2">"sh ${sync_shell} "&amp;E6&amp;" ${dt}"</f>
         <v>sh ${sync_shell} flow_c ${dt}</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I7" s="5" t="str">
-        <f t="shared" ref="I7" si="4">E6</f>
+        <f t="shared" ref="I7" si="3">E6</f>
         <v>flow_c</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" ref="E8" si="5">LOWER(B8)</f>
+        <f t="shared" ref="E8" si="4">LOWER(B8)</f>
         <v>flow_d</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8" si="6">"sh ${sync_shell} "&amp;E8&amp;" ${dt}"</f>
+        <f t="shared" ref="H8" si="5">"sh ${sync_shell} "&amp;E8&amp;" ${dt}"</f>
         <v>sh ${sync_shell} flow_d ${dt}</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I9" s="5" t="str">
-        <f t="shared" ref="I9" si="7">E8</f>
+        <f t="shared" ref="I9" si="6">E8</f>
         <v>flow_d</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ref="E10" si="8">LOWER(B10)</f>
+        <f t="shared" ref="E10" si="7">LOWER(B10)</f>
         <v>flow_e</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="5" t="str">
-        <f t="shared" ref="H10" si="9">"sh ${sync_shell} "&amp;E10&amp;" ${dt}"</f>
+        <f t="shared" ref="H10" si="8">"sh ${sync_shell} "&amp;E10&amp;" ${dt}"</f>
         <v>sh ${sync_shell} flow_e ${dt}</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I11" s="5" t="str">
-        <f t="shared" ref="I11" si="10">E10</f>
+        <f t="shared" ref="I11" si="9">E10</f>
         <v>flow_e</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" ref="E12" si="11">LOWER(B12)</f>
+        <f t="shared" ref="E12" si="10">LOWER(B12)</f>
         <v>flow_f</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="5" t="str">
-        <f t="shared" ref="H12" si="12">"sh ${sync_shell} "&amp;E12&amp;" ${dt}"</f>
+        <f t="shared" ref="H12" si="11">"sh ${sync_shell} "&amp;E12&amp;" ${dt}"</f>
         <v>sh ${sync_shell} flow_f ${dt}</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I13" s="5" t="str">
-        <f t="shared" ref="I13" si="13">E12</f>
+        <f t="shared" ref="I13" si="12">E12</f>
         <v>flow_f</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="5" t="str">
         <f>"sh ${check_script} ora2pg "&amp;UPPER(MID(E14,7,6)&amp;" ${dt}")</f>
@@ -2182,118 +2757,118 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="5" t="str">
-        <f t="shared" ref="H15:H19" si="14">"sh ${check_script} ora2pg "&amp;UPPER(MID(E15,7,6)&amp;" ${dt}")</f>
+        <f t="shared" ref="H15:H19" si="13">"sh ${check_script} ora2pg "&amp;UPPER(MID(E15,7,6)&amp;" ${dt}")</f>
         <v>sh ${check_script} ora2pg FLOW_B ${DT}</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>sh ${check_script} ora2pg FLOW_C ${DT}</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>sh ${check_script} ora2pg FLOW_D ${DT}</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>sh ${check_script} ora2pg FLOW_E ${DT}</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>sh ${check_script} ora2pg FLOW_F ${DT}</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename  repo name azkaban_excel_yaml to azkaban_helper
</commit_message>
<xml_diff>
--- a/docs/template.xlsx
+++ b/docs/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jing/PycharmProjects/azkaban_excel_yaml/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73986CE7-9726-2E46-A00D-9B3461BD2739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E28D7B9-E127-F041-925C-8ECE7C789AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="91">
   <si>
     <t>Overview</t>
   </si>
@@ -343,22 +343,10 @@
     <t>desc</t>
   </si>
   <si>
-    <t>https://192.168.200.100:8443/</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>G:\tmp\azkaban\</t>
-  </si>
-  <si>
-    <t>window test env</t>
-  </si>
-  <si>
     <t>/Users/jing/jbf/jobs</t>
-  </si>
-  <si>
-    <t>local devlop env</t>
   </si>
   <si>
     <t>project_name</t>
@@ -554,18 +542,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>su - pg -c "sh ${create_script} ora4pg ${azkaban.flow.flowid} ${dt}"</t>
-  </si>
-  <si>
-    <t>su - pg -c "sh ${create_script} ora5pg ${azkaban.flow.flowid} ${dt}"</t>
-  </si>
-  <si>
-    <t>su - pg -c "sh ${create_script} ora6pg ${azkaban.flow.flowid} ${dt}"</t>
-  </si>
-  <si>
-    <t>su - pg -c "sh ${create_script} ora7pg ${azkaban.flow.flowid} ${dt}"</t>
-  </si>
-  <si>
     <t>check_flow_a</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -615,6 +591,134 @@
   <si>
     <t>1.0.0</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project URL</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/JingZhang-Cherish/azkaban_excel_yaml</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>sla_enabled</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>sla_emails</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flow/job</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>rule</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>email_action</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>kill_action</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1126199037@qq.com</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>durtion(HH:MM)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:02</t>
+  </si>
+  <si>
+    <t>00:03</t>
+  </si>
+  <si>
+    <t>00:04</t>
+  </si>
+  <si>
+    <t>00:05</t>
+  </si>
+  <si>
+    <t>00:06</t>
+  </si>
+  <si>
+    <t>00:07</t>
+  </si>
+  <si>
+    <t>https://192.168.31.36:18443/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>1126199037@qq.com;244612023@qq.com</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>echo bbb</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>echo bbb_done</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flowPriority=50|sync_shell=/home/pg/tools/migration/gil/sync_data.sh|</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>00:02</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>su - pg -c "sh ${create_script} ora2pg ${azkaban.flow.flowid} ${dt}"</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flowPriority=50|sync_shell=/home/pg/tools/migration/gil/sync_data.sh</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>su -pg -c "sh check_flow_status.sh ${azkaban.flow.execid} ${dt}"</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://100.65.87.14:8443/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhfd 云测试环境</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地环境</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://100.65.87.19:8443/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhfd 云生产环境</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://100.65.87.20:8443/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhfd 云生产环境(备)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://192.168.31.36:18443/</t>
   </si>
   <si>
     <r>
@@ -653,97 +757,8 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>more detail read READMI.md on github or pypi</t>
+      <t>more detail read README.md on github or pypi</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project URL</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://github.com/JingZhang-Cherish/azkaban_excel_yaml</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>sla_enabled</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>sla_emails</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Flow/job</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>rule</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>email_action</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>kill_action</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>1126199037@qq.com</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>SUCCESS</t>
-  </si>
-  <si>
-    <t>durtion(HH:MM)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>00:02</t>
-  </si>
-  <si>
-    <t>00:03</t>
-  </si>
-  <si>
-    <t>00:04</t>
-  </si>
-  <si>
-    <t>00:05</t>
-  </si>
-  <si>
-    <t>00:06</t>
-  </si>
-  <si>
-    <t>00:07</t>
-  </si>
-  <si>
-    <t>https://192.168.31.36:18443/</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>1126199037@qq.com;244612023@qq.com</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>echo bbb</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>echo bbb_done</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>flowPriority=50|sync_shell=/home/pg/tools/migration/gil/sync_data.sh|</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>flowPriority=50|sync_shell=/home/pg/tools/migration/gil/sync_data.sh|failure.emails=244612023@qq.com</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>00:02</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -754,7 +769,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,6 +860,12 @@
       <color rgb="FF000000"/>
       <name val="Microsoft YaHei UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1062,8 +1083,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1079,13 +1101,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1359,7 +1432,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -1374,29 +1447,29 @@
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="44" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="17"/>
       <c r="B3" s="28" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16">
@@ -1416,10 +1489,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="23">
         <v>44463</v>
@@ -1430,10 +1503,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="D6" s="23">
         <v>44469</v>
@@ -1479,7 +1552,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1488,13 +1561,13 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16">
+    <row r="1" spans="1:7" ht="16">
       <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
@@ -1511,50 +1584,94 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="str">
+        <f>VLOOKUP(A2,A3:B100,2,FALSE)</f>
+        <v>本地环境</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
+      <c r="B6" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="本地">
+      <formula>NOT(ISERROR(SEARCH("本地",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="生产">
+      <formula>NOT(ISERROR(SEARCH("生产",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="本地">
+      <formula>NOT(ISERROR(SEARCH("本地",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="生产">
+      <formula>NOT(ISERROR(SEARCH("生产",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{CFDDEEB9-25D5-BC47-BF56-EC874F5819DE}">
+      <formula1>$A$6:$A$79</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6B8E32BD-1905-7C41-BB26-21970D225511}"/>
   </hyperlinks>
@@ -1578,21 +1695,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1627,7 +1744,7 @@
   <dimension ref="A1:N98"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
@@ -1639,65 +1756,65 @@
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="30" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="N1" s="30" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="24" t="str">
         <f>G2&amp;" "&amp;F2&amp;" "&amp;E2&amp;" ? * *"</f>
@@ -1716,20 +1833,20 @@
         <v>0</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J8" si="0">B2</f>
         <v>FLOW_A</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -1740,10 +1857,10 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" s="24" t="str">
         <f t="shared" ref="C3:C8" si="1">G3&amp;" "&amp;F3&amp;" "&amp;E3&amp;" ? * *"</f>
@@ -1765,17 +1882,17 @@
         <v>0</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
         <v>FLOW_B</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
@@ -1786,10 +1903,10 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C4" s="24" t="str">
         <f t="shared" si="1"/>
@@ -1811,17 +1928,17 @@
         <v>0</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>FLOW_C</v>
       </c>
       <c r="K4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -1832,10 +1949,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" s="24" t="str">
         <f t="shared" si="1"/>
@@ -1857,17 +1974,17 @@
         <v>0</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
         <v>FLOW_D</v>
       </c>
       <c r="K5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -1878,10 +1995,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="24" t="str">
         <f t="shared" si="1"/>
@@ -1903,17 +2020,17 @@
         <v>0</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
         <v>FLOW_E</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L6" s="31" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -1924,10 +2041,10 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7" s="24" t="str">
         <f t="shared" si="1"/>
@@ -1949,17 +2066,17 @@
         <v>0</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
         <v>FLOW_F</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -1970,10 +2087,10 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C8" s="24" t="str">
         <f t="shared" si="1"/>
@@ -1995,17 +2112,17 @@
         <v>0</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
         <v>FLOW_DONE</v>
       </c>
       <c r="K8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L8" s="31" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -2418,10 +2535,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="39.83203125" defaultRowHeight="15"/>
@@ -2439,68 +2556,67 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>87</v>
+        <v>40</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>80</v>
       </c>
       <c r="E2" t="str">
         <f>LOWER(B2)</f>
         <v>flow_a</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="5" t="str">
-        <f>"sleep 200"</f>
-        <v>sleep 200</v>
+        <v>27</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H3" s="5" t="str">
         <f>"sleep 1"</f>
@@ -2513,13 +2629,13 @@
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1">
       <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>86</v>
+      <c r="D4" s="33" t="s">
+        <v>77</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ref="E4" si="0">LOWER(B4)</f>
@@ -2527,31 +2643,31 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="11"/>
       <c r="E5" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I5" s="5" t="str">
         <f>E4</f>
@@ -2560,20 +2676,20 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ref="E6" si="1">LOWER(B6)</f>
         <v>flow_c</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H6" s="5" t="str">
         <f t="shared" ref="H6" si="2">"sh ${sync_shell} "&amp;E6&amp;" ${dt}"</f>
@@ -2582,20 +2698,20 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="I7" s="5" t="str">
         <f t="shared" ref="I7" si="3">E6</f>
@@ -2604,20 +2720,20 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" ref="E8" si="4">LOWER(B8)</f>
         <v>flow_d</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H8" s="5" t="str">
         <f t="shared" ref="H8" si="5">"sh ${sync_shell} "&amp;E8&amp;" ${dt}"</f>
@@ -2626,20 +2742,20 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="I9" s="5" t="str">
         <f t="shared" ref="I9" si="6">E8</f>
@@ -2648,20 +2764,20 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ref="E10" si="7">LOWER(B10)</f>
         <v>flow_e</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H10" s="5" t="str">
         <f t="shared" ref="H10" si="8">"sh ${sync_shell} "&amp;E10&amp;" ${dt}"</f>
@@ -2670,20 +2786,20 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>52</v>
+        <v>27</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="I11" s="5" t="str">
         <f t="shared" ref="I11" si="9">E10</f>
@@ -2692,20 +2808,20 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" ref="E12" si="10">LOWER(B12)</f>
         <v>flow_f</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H12" s="5" t="str">
         <f t="shared" ref="H12" si="11">"sh ${sync_shell} "&amp;E12&amp;" ${dt}"</f>
@@ -2714,20 +2830,20 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="I13" s="5" t="str">
         <f t="shared" ref="I13" si="12">E12</f>
@@ -2736,140 +2852,143 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H14" s="5" t="str">
-        <f>"sh ${check_script} ora2pg "&amp;UPPER(MID(E14,7,6)&amp;" ${dt}")</f>
-        <v>sh ${check_script} ora2pg FLOW_A ${DT}</v>
+        <f>"sh ${check_script} ora2pg "&amp;UPPER(MID(E14,7,6))&amp;" ${dt}"</f>
+        <v>sh ${check_script} ora2pg FLOW_A ${dt}</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H15" s="5" t="str">
-        <f t="shared" ref="H15:H19" si="13">"sh ${check_script} ora2pg "&amp;UPPER(MID(E15,7,6)&amp;" ${dt}")</f>
-        <v>sh ${check_script} ora2pg FLOW_B ${DT}</v>
+        <f t="shared" ref="H15:H19" si="13">"sh ${check_script} ora2pg "&amp;UPPER(MID(E15,7,6))&amp;" ${dt}"</f>
+        <v>sh ${check_script} ora2pg FLOW_B ${dt}</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H16" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>sh ${check_script} ora2pg FLOW_C ${DT}</v>
+        <v>sh ${check_script} ora2pg FLOW_C ${dt}</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H17" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>sh ${check_script} ora2pg FLOW_D ${DT}</v>
+        <v>sh ${check_script} ora2pg FLOW_D ${dt}</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H18" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>sh ${check_script} ora2pg FLOW_E ${DT}</v>
+        <v>sh ${check_script} ora2pg FLOW_E ${dt}</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H19" s="5" t="str">
         <f t="shared" si="13"/>
-        <v>sh ${check_script} ora2pg FLOW_F ${DT}</v>
+        <v>sh ${check_script} ora2pg FLOW_F ${dt}</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="I20" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18">
+      <c r="E24" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>